<commit_message>
Many new small implementation
</commit_message>
<xml_diff>
--- a/ImplementedFeatures.xlsx
+++ b/ImplementedFeatures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="GSettings" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="GVariantType" sheetId="4" r:id="rId3"/>
     <sheet name="GVariant" sheetId="2" r:id="rId4"/>
     <sheet name="GString" sheetId="5" r:id="rId5"/>
-    <sheet name="GSettingsSchema" sheetId="6" r:id="rId6"/>
+    <sheet name="GSettingsSchemaSource" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="342">
   <si>
     <t>GSettings *</t>
   </si>
@@ -1037,6 +1037,24 @@
   </si>
   <si>
     <t>Todo</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>schemaKey</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>poc</t>
+  </si>
+  <si>
+    <t>still require official test</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1179,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -1205,7 +1223,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1493,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4420,10 +4439,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4432,260 +4451,341 @@
     <col min="3" max="3" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="16"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="E3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="E4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="E5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C6" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="E6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C7" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="E7" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="E8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="E10" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="E11" t="s">
+        <v>337</v>
+      </c>
+      <c r="F11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="E12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="E13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="E14" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="E15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C16" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E16" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E17" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="E18" t="s">
+        <v>337</v>
+      </c>
+      <c r="F18" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="E20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="E21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="E22" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C23" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="E23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D12" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D13" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D14" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D15" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="D16" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="D17" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D19" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="D20" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="D21" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D22" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D23" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="9" t="s">
         <v>333</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
+      <c r="E24" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="9" t="s">
         <v>334</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>335</v>
+      </c>
+      <c r="E25" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -4722,5 +4822,6 @@
     <hyperlink ref="C25" r:id="rId30" location="g-settings-schema-key-get-description" tooltip="g_settings_schema_key_get_description ()" display="https://developer.gnome.org/gio/stable/gio-GSettingsSchema-GSettingsSchemaSource.html - g-settings-schema-key-get-description"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update readme and code partly
</commit_message>
<xml_diff>
--- a/ImplementedFeatures.xlsx
+++ b/ImplementedFeatures.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GSettings" sheetId="1" r:id="rId1"/>
-    <sheet name="GAction" sheetId="3" r:id="rId2"/>
-    <sheet name="GVariantType" sheetId="4" r:id="rId3"/>
-    <sheet name="GVariant" sheetId="2" r:id="rId4"/>
-    <sheet name="GString" sheetId="5" r:id="rId5"/>
-    <sheet name="GSettingsSchemaSource" sheetId="6" r:id="rId6"/>
+    <sheet name="GSettingsBackend" sheetId="7" r:id="rId2"/>
+    <sheet name="GAction" sheetId="3" r:id="rId3"/>
+    <sheet name="GVariantType" sheetId="4" r:id="rId4"/>
+    <sheet name="GVariant" sheetId="2" r:id="rId5"/>
+    <sheet name="GString" sheetId="5" r:id="rId6"/>
+    <sheet name="GSettingsSchemaSource" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="342">
   <si>
     <t>GSettings *</t>
   </si>
@@ -238,27 +239,15 @@
     <t>X</t>
   </si>
   <si>
-    <t>Missing the Gvariant class</t>
-  </si>
-  <si>
     <t>Require tests</t>
   </si>
   <si>
     <t>Tested</t>
   </si>
   <si>
-    <t>Bad implementation, missing Gvariant class</t>
-  </si>
-  <si>
-    <t>No tests, and expected to fails. (Also obsolete)</t>
-  </si>
-  <si>
     <t>Missing backend</t>
   </si>
   <si>
-    <t>Bad implementation, missing Gvariant class (Deprecated)</t>
-  </si>
-  <si>
     <t>I don't understand how it works</t>
   </si>
   <si>
@@ -1058,6 +1047,15 @@
   </si>
   <si>
     <t>tested by using compare</t>
+  </si>
+  <si>
+    <t>https://developer.gnome.org/gio/stable/GSettingsBackend.html</t>
+  </si>
+  <si>
+    <t>Obsolete</t>
+  </si>
+  <si>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1180,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -1228,6 +1226,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1515,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1524,6 +1523,7 @@
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="46.77734375" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1535,10 +1535,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
@@ -1549,10 +1549,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
@@ -1563,7 +1563,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1574,7 +1574,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -1593,35 +1593,29 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -1632,7 +1626,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
@@ -1643,7 +1637,7 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
@@ -1654,7 +1648,7 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
@@ -1665,7 +1659,7 @@
         <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -1676,7 +1670,7 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
@@ -1687,7 +1681,7 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
@@ -1698,35 +1692,29 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="13" t="s">
+      <c r="B18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -1737,10 +1725,10 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" t="s">
-        <v>308</v>
+        <v>76</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -1751,10 +1739,10 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -1765,7 +1753,10 @@
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
@@ -1776,7 +1767,7 @@
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
@@ -1787,10 +1778,10 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" t="s">
         <v>75</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
@@ -1801,10 +1792,10 @@
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" t="s">
         <v>75</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
@@ -1818,7 +1809,7 @@
         <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
@@ -1832,7 +1823,7 @@
         <v>68</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
@@ -1843,7 +1834,7 @@
         <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
@@ -1854,7 +1845,7 @@
         <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
@@ -1865,7 +1856,7 @@
         <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
@@ -1876,7 +1867,7 @@
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
@@ -1887,7 +1878,7 @@
         <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
@@ -1898,7 +1889,7 @@
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -1909,7 +1900,7 @@
         <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
@@ -1920,7 +1911,7 @@
         <v>41</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
@@ -1931,7 +1922,7 @@
         <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
@@ -1942,7 +1933,7 @@
         <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
@@ -1953,7 +1944,7 @@
         <v>46</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
@@ -1964,7 +1955,7 @@
         <v>47</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
@@ -1975,7 +1966,7 @@
         <v>49</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
@@ -1986,7 +1977,7 @@
         <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
@@ -1997,7 +1988,7 @@
         <v>51</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
@@ -2008,7 +1999,7 @@
         <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
@@ -2019,7 +2010,7 @@
         <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
@@ -2030,7 +2021,7 @@
         <v>54</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
@@ -2041,7 +2032,7 @@
         <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
@@ -2052,7 +2043,7 @@
         <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
@@ -2127,7 +2118,7 @@
         <v>67</v>
       </c>
       <c r="D55" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2201,6 +2192,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2219,43 +2233,43 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
@@ -2263,10 +2277,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
@@ -2274,10 +2288,10 @@
         <v>10</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
@@ -2285,10 +2299,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
@@ -2296,10 +2310,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
         <v>91</v>
-      </c>
-      <c r="D9" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
@@ -2307,10 +2321,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
@@ -2318,10 +2332,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
@@ -2329,10 +2343,10 @@
         <v>48</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2353,12 +2367,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C31"/>
+  <dimension ref="B2:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2367,124 +2381,130 @@
     <col min="3" max="3" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="D6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C5" s="7" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="9" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="9" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -2492,7 +2512,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
@@ -2500,7 +2520,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
@@ -2508,7 +2528,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
@@ -2516,7 +2536,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
@@ -2524,87 +2544,87 @@
         <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2672,11 +2692,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -2695,7 +2715,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2706,7 +2726,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2717,7 +2737,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2728,7 +2748,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2736,15 +2756,15 @@
         <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2752,10 +2772,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2766,7 +2786,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -2777,7 +2797,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -2788,10 +2808,10 @@
         <v>33</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2799,10 +2819,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2813,7 +2833,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2824,7 +2844,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2835,7 +2855,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2846,7 +2866,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2857,7 +2877,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2868,7 +2888,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2879,7 +2899,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2890,7 +2910,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2901,7 +2921,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2912,10 +2932,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2926,7 +2946,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2937,10 +2957,10 @@
         <v>8</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2951,7 +2971,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2962,10 +2982,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2976,7 +2996,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2987,10 +3007,10 @@
         <v>8</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -3001,10 +3021,10 @@
         <v>8</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -3015,10 +3035,10 @@
         <v>8</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -3029,10 +3049,10 @@
         <v>8</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D31" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -3043,7 +3063,7 @@
         <v>10</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3054,10 +3074,10 @@
         <v>8</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D33" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3068,7 +3088,7 @@
         <v>10</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -3079,7 +3099,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -3090,10 +3110,10 @@
         <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D36" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -3104,7 +3124,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -3115,10 +3135,10 @@
         <v>8</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D38" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -3129,7 +3149,7 @@
         <v>8</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -3140,7 +3160,7 @@
         <v>10</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -3148,10 +3168,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -3159,10 +3179,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -3170,10 +3190,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3181,10 +3201,10 @@
         <v>1</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -3192,10 +3212,10 @@
         <v>1</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -3206,7 +3226,7 @@
         <v>36</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -3217,7 +3237,7 @@
         <v>42</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -3225,10 +3245,10 @@
         <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -3239,7 +3259,7 @@
         <v>45</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -3247,10 +3267,10 @@
         <v>2</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -3261,7 +3281,7 @@
         <v>48</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -3272,7 +3292,7 @@
         <v>8</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -3280,10 +3300,10 @@
         <v>2</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -3294,7 +3314,7 @@
         <v>24</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -3302,10 +3322,10 @@
         <v>2</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -3316,7 +3336,7 @@
         <v>24</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -3324,10 +3344,10 @@
         <v>2</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -3338,7 +3358,7 @@
         <v>48</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -3346,10 +3366,10 @@
         <v>2</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -3360,7 +3380,7 @@
         <v>24</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -3371,10 +3391,10 @@
         <v>8</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D61" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -3382,10 +3402,10 @@
         <v>8</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D62" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -3393,10 +3413,10 @@
         <v>8</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D63" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -3404,7 +3424,7 @@
         <v>8</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
@@ -3412,7 +3432,7 @@
         <v>8</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
@@ -3420,18 +3440,18 @@
         <v>8</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D67" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
@@ -3439,7 +3459,7 @@
         <v>8</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
@@ -3447,7 +3467,7 @@
         <v>6</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
@@ -3455,7 +3475,7 @@
         <v>8</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
@@ -3463,42 +3483,42 @@
         <v>10</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" s="8" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D75" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
@@ -3506,7 +3526,7 @@
         <v>6</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
@@ -3514,7 +3534,7 @@
         <v>8</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
@@ -3522,7 +3542,7 @@
         <v>8</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
@@ -3530,7 +3550,7 @@
         <v>8</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
@@ -3538,7 +3558,7 @@
         <v>8</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -3546,7 +3566,7 @@
         <v>10</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -3554,7 +3574,7 @@
         <v>39</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -3562,7 +3582,7 @@
         <v>10</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -3573,23 +3593,23 @@
         <v>48</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B85" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -3597,31 +3617,31 @@
         <v>6</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -3629,7 +3649,7 @@
         <v>8</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -3637,7 +3657,7 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -3645,15 +3665,15 @@
         <v>10</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -3661,23 +3681,23 @@
         <v>6</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.3">
@@ -3685,7 +3705,7 @@
         <v>6</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.3">
@@ -3693,7 +3713,7 @@
         <v>6</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.3">
@@ -3701,7 +3721,7 @@
         <v>6</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.3">
@@ -3709,7 +3729,7 @@
         <v>6</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.3">
@@ -3717,7 +3737,7 @@
         <v>6</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.3">
@@ -3725,7 +3745,7 @@
         <v>8</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.3">
@@ -3733,7 +3753,7 @@
         <v>6</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.3">
@@ -3741,15 +3761,15 @@
         <v>6</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.3">
@@ -3757,23 +3777,23 @@
         <v>6</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.3">
@@ -3781,7 +3801,7 @@
         <v>6</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.3">
@@ -3789,7 +3809,7 @@
         <v>6</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.3">
@@ -3797,7 +3817,7 @@
         <v>10</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.3">
@@ -3805,7 +3825,7 @@
         <v>10</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.3">
@@ -3813,7 +3833,7 @@
         <v>8</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.3">
@@ -3821,7 +3841,7 @@
         <v>6</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.3">
@@ -3829,7 +3849,7 @@
         <v>6</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.3">
@@ -3837,7 +3857,7 @@
         <v>10</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.3">
@@ -3845,7 +3865,7 @@
         <v>8</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.3">
@@ -3853,7 +3873,7 @@
         <v>8</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.3">
@@ -3861,7 +3881,7 @@
         <v>8</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.3">
@@ -3869,7 +3889,7 @@
         <v>8</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.3">
@@ -3877,7 +3897,7 @@
         <v>48</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4108,12 +4128,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4124,34 +4144,34 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -4159,7 +4179,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
@@ -4167,7 +4187,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
@@ -4175,7 +4195,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
@@ -4183,151 +4203,151 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
@@ -4335,31 +4355,31 @@
         <v>48</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
@@ -4367,7 +4387,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
@@ -4375,7 +4395,7 @@
         <v>10</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4446,7 +4466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -4465,30 +4485,30 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E4" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4496,27 +4516,27 @@
         <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>313</v>
-      </c>
       <c r="D6" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E6" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -4524,44 +4544,44 @@
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E8" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F8" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E9" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -4569,47 +4589,47 @@
         <v>6</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E10" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E11" t="s">
+        <v>333</v>
+      </c>
+      <c r="F11" t="s">
         <v>337</v>
-      </c>
-      <c r="F11" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E12" t="s">
+        <v>333</v>
+      </c>
+      <c r="F12" t="s">
         <v>337</v>
-      </c>
-      <c r="F12" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -4617,41 +4637,41 @@
         <v>10</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E13" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E14" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E15" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -4659,13 +4679,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E16" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
@@ -4673,13 +4693,13 @@
         <v>24</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E17" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
@@ -4687,30 +4707,30 @@
         <v>24</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E18" t="s">
+        <v>333</v>
+      </c>
+      <c r="F18" t="s">
         <v>337</v>
-      </c>
-      <c r="F18" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E19" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
@@ -4718,13 +4738,13 @@
         <v>8</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E20" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
@@ -4732,13 +4752,13 @@
         <v>8</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E21" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
@@ -4746,55 +4766,55 @@
         <v>10</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>335</v>
-      </c>
       <c r="E22" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E23" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E24" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="E25" t="s">
         <v>334</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="E25" t="s">
-        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the libgio-2.0.so for libgio-2.0.so.0
</commit_message>
<xml_diff>
--- a/ImplementedFeatures.xlsx
+++ b/ImplementedFeatures.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GSettings" sheetId="1" r:id="rId1"/>
     <sheet name="GSettingsBackend" sheetId="7" r:id="rId2"/>
     <sheet name="GAction" sheetId="3" r:id="rId3"/>
     <sheet name="GVariantType" sheetId="4" r:id="rId4"/>
-    <sheet name="GVariant" sheetId="2" r:id="rId5"/>
-    <sheet name="GString" sheetId="5" r:id="rId6"/>
-    <sheet name="GSettingsSchemaSource" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
+    <sheet name="GVariant" sheetId="2" r:id="rId6"/>
+    <sheet name="GString" sheetId="5" r:id="rId7"/>
+    <sheet name="GSettingsSchemaSource" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="345">
   <si>
     <t>GSettings *</t>
   </si>
@@ -1056,6 +1057,15 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>https://developer.gnome.org/dbus-glib/unstable/dbus-glib-DBusGConnection.html#dbus-g-bus-get</t>
+  </si>
+  <si>
+    <t>dbus_g_connection_register_g_object ()</t>
+  </si>
+  <si>
+    <t>libdbus-glib-1.so.2</t>
   </si>
 </sst>
 </file>
@@ -1518,16 +1528,16 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="46.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1541,7 +1551,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1565,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +1576,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1577,7 +1587,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
@@ -1596,7 +1606,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
@@ -1607,7 +1617,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
@@ -1618,7 +1628,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1629,7 +1639,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
@@ -1640,7 +1650,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
@@ -1662,7 +1672,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
@@ -1673,7 +1683,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>0</v>
       </c>
@@ -1684,7 +1694,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
@@ -1695,7 +1705,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>8</v>
       </c>
@@ -1706,7 +1716,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
@@ -1717,7 +1727,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>21</v>
       </c>
@@ -1731,7 +1741,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
@@ -1745,7 +1755,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>24</v>
       </c>
@@ -1759,7 +1769,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>24</v>
       </c>
@@ -1770,7 +1780,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
@@ -1784,7 +1794,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>10</v>
       </c>
@@ -1798,7 +1808,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>6</v>
       </c>
@@ -1812,7 +1822,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>10</v>
       </c>
@@ -1826,7 +1836,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
@@ -1837,7 +1847,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>10</v>
       </c>
@@ -1848,7 +1858,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>33</v>
       </c>
@@ -1859,7 +1869,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>10</v>
       </c>
@@ -1870,7 +1880,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>36</v>
       </c>
@@ -1881,7 +1891,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>10</v>
       </c>
@@ -1892,7 +1902,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>39</v>
       </c>
@@ -1903,7 +1913,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>10</v>
       </c>
@@ -1914,7 +1924,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>42</v>
       </c>
@@ -1925,7 +1935,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>10</v>
       </c>
@@ -1936,7 +1946,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>45</v>
       </c>
@@ -1947,7 +1957,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>10</v>
       </c>
@@ -1958,7 +1968,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>48</v>
       </c>
@@ -1969,7 +1979,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>10</v>
       </c>
@@ -1980,7 +1990,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
         <v>24</v>
       </c>
@@ -1991,7 +2001,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2012,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>33</v>
       </c>
@@ -2013,7 +2023,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>10</v>
       </c>
@@ -2024,7 +2034,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>39</v>
       </c>
@@ -2035,7 +2045,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>10</v>
       </c>
@@ -2046,7 +2056,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
         <v>10</v>
       </c>
@@ -2054,7 +2064,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="12" t="s">
         <v>58</v>
       </c>
@@ -2062,7 +2072,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
         <v>6</v>
       </c>
@@ -2070,7 +2080,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
         <v>6</v>
       </c>
@@ -2078,7 +2088,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="s">
         <v>6</v>
       </c>
@@ -2086,7 +2096,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="12" t="s">
         <v>6</v>
       </c>
@@ -2094,7 +2104,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
         <v>8</v>
       </c>
@@ -2102,7 +2112,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
         <v>10</v>
       </c>
@@ -2110,7 +2120,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>66</v>
       </c>
@@ -2198,9 +2208,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>339</v>
       </c>
@@ -2221,14 +2231,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.109375" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
@@ -2239,7 +2249,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>79</v>
       </c>
@@ -2250,7 +2260,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>81</v>
       </c>
@@ -2261,7 +2271,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>81</v>
       </c>
@@ -2272,7 +2282,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
@@ -2283,7 +2293,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
@@ -2294,7 +2304,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
@@ -2305,7 +2315,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -2316,7 +2326,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
@@ -2327,7 +2337,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
@@ -2338,7 +2348,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>48</v>
       </c>
@@ -2371,17 +2381,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>197</v>
       </c>
@@ -2389,7 +2399,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
@@ -2397,7 +2407,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>231</v>
       </c>
@@ -2405,7 +2415,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>231</v>
       </c>
@@ -2413,7 +2423,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
@@ -2424,7 +2434,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2435,7 +2445,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>165</v>
       </c>
@@ -2443,7 +2453,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>79</v>
       </c>
@@ -2451,7 +2461,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>48</v>
       </c>
@@ -2459,7 +2469,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
@@ -2467,7 +2477,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
@@ -2475,7 +2485,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
@@ -2483,7 +2493,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
@@ -2491,7 +2501,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
@@ -2499,7 +2509,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
@@ -2507,7 +2517,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>10</v>
       </c>
@@ -2515,7 +2525,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>10</v>
       </c>
@@ -2523,7 +2533,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>39</v>
       </c>
@@ -2531,7 +2541,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>10</v>
       </c>
@@ -2539,7 +2549,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>10</v>
       </c>
@@ -2547,7 +2557,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>231</v>
       </c>
@@ -2555,7 +2565,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>231</v>
       </c>
@@ -2563,7 +2573,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>231</v>
       </c>
@@ -2571,7 +2581,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>231</v>
       </c>
@@ -2579,7 +2589,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>81</v>
       </c>
@@ -2587,7 +2597,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>165</v>
       </c>
@@ -2595,7 +2605,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>81</v>
       </c>
@@ -2603,7 +2613,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
         <v>81</v>
       </c>
@@ -2611,7 +2621,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
         <v>81</v>
       </c>
@@ -2619,7 +2629,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>81</v>
       </c>
@@ -2694,20 +2704,54 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="dbus-g-bus-get" display="https://developer.gnome.org/dbus-glib/unstable/dbus-glib-DBusGConnection.html - dbus-g-bus-get"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="66.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2718,7 +2762,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2729,7 +2773,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2740,7 +2784,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2751,7 +2795,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
@@ -2759,7 +2803,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>81</v>
       </c>
@@ -2767,7 +2811,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2778,7 +2822,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2789,7 +2833,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2800,7 +2844,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2814,7 +2858,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2825,7 +2869,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2836,7 +2880,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2847,7 +2891,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2858,7 +2902,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2869,7 +2913,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2880,7 +2924,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2891,7 +2935,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2902,7 +2946,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2913,7 +2957,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2924,7 +2968,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2938,7 +2982,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2949,7 +2993,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2963,7 +3007,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2974,7 +3018,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2988,7 +3032,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2999,7 +3043,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3013,7 +3057,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -3027,7 +3071,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -3041,7 +3085,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -3055,7 +3099,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -3066,7 +3110,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -3080,7 +3124,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3091,7 +3135,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -3102,7 +3146,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -3116,7 +3160,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -3127,7 +3171,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -3141,7 +3185,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -3152,7 +3196,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -3163,7 +3207,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3174,7 +3218,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3185,7 +3229,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3196,7 +3240,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3207,7 +3251,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3218,7 +3262,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3229,7 +3273,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -3240,7 +3284,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -3251,7 +3295,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3262,7 +3306,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2</v>
       </c>
@@ -3273,7 +3317,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -3284,7 +3328,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -3295,7 +3339,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3306,7 +3350,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -3317,7 +3361,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
@@ -3328,7 +3372,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -3339,7 +3383,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -3350,7 +3394,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -3361,7 +3405,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -3372,7 +3416,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -3383,7 +3427,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -3397,7 +3441,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="12" t="s">
         <v>8</v>
       </c>
@@ -3408,7 +3452,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>8</v>
       </c>
@@ -3419,7 +3463,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>8</v>
       </c>
@@ -3427,7 +3471,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
@@ -3435,7 +3479,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="8" t="s">
         <v>8</v>
       </c>
@@ -3443,7 +3487,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>165</v>
       </c>
@@ -3454,7 +3498,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>8</v>
       </c>
@@ -3462,7 +3506,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>6</v>
       </c>
@@ -3470,7 +3514,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
         <v>8</v>
       </c>
@@ -3478,7 +3522,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>10</v>
       </c>
@@ -3486,7 +3530,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>171</v>
       </c>
@@ -3494,7 +3538,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="8" t="s">
         <v>165</v>
       </c>
@@ -3502,7 +3546,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>171</v>
       </c>
@@ -3510,7 +3554,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="8" t="s">
         <v>175</v>
       </c>
@@ -3521,7 +3565,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>6</v>
       </c>
@@ -3529,7 +3573,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>8</v>
       </c>
@@ -3537,7 +3581,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>8</v>
       </c>
@@ -3545,7 +3589,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="8" t="s">
         <v>8</v>
       </c>
@@ -3553,7 +3597,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="s">
         <v>8</v>
       </c>
@@ -3561,7 +3605,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>10</v>
       </c>
@@ -3569,7 +3613,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B82" s="8" t="s">
         <v>39</v>
       </c>
@@ -3577,7 +3621,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B83" s="8" t="s">
         <v>10</v>
       </c>
@@ -3585,7 +3629,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1</v>
       </c>
@@ -3596,7 +3640,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" s="6" t="s">
         <v>186</v>
       </c>
@@ -3604,7 +3648,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>188</v>
       </c>
@@ -3612,7 +3656,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
         <v>6</v>
       </c>
@@ -3620,7 +3664,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>165</v>
       </c>
@@ -3628,7 +3672,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>165</v>
       </c>
@@ -3636,7 +3680,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>188</v>
       </c>
@@ -3644,7 +3688,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>8</v>
       </c>
@@ -3652,7 +3696,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>10</v>
       </c>
@@ -3660,7 +3704,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>10</v>
       </c>
@@ -3668,7 +3712,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
         <v>197</v>
       </c>
@@ -3676,7 +3720,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>6</v>
       </c>
@@ -3684,7 +3728,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>200</v>
       </c>
@@ -3692,7 +3736,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>200</v>
       </c>
@@ -3700,7 +3744,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
         <v>6</v>
       </c>
@@ -3708,7 +3752,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
         <v>6</v>
       </c>
@@ -3716,7 +3760,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="3" t="s">
         <v>6</v>
       </c>
@@ -3724,7 +3768,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
         <v>6</v>
       </c>
@@ -3732,7 +3776,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
         <v>6</v>
       </c>
@@ -3740,7 +3784,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>8</v>
       </c>
@@ -3748,7 +3792,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
         <v>6</v>
       </c>
@@ -3756,7 +3800,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
         <v>6</v>
       </c>
@@ -3764,7 +3808,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
         <v>197</v>
       </c>
@@ -3772,7 +3816,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
         <v>6</v>
       </c>
@@ -3780,7 +3824,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
         <v>213</v>
       </c>
@@ -3788,7 +3832,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
         <v>213</v>
       </c>
@@ -3796,7 +3840,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
         <v>6</v>
       </c>
@@ -3804,7 +3848,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
         <v>6</v>
       </c>
@@ -3812,7 +3856,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
         <v>10</v>
       </c>
@@ -3820,7 +3864,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
         <v>10</v>
       </c>
@@ -3828,7 +3872,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
         <v>8</v>
       </c>
@@ -3836,7 +3880,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
         <v>6</v>
       </c>
@@ -3844,7 +3888,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
         <v>6</v>
       </c>
@@ -3852,7 +3896,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
         <v>10</v>
       </c>
@@ -3860,7 +3904,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
         <v>8</v>
       </c>
@@ -3868,7 +3912,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
         <v>8</v>
       </c>
@@ -3876,7 +3920,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
         <v>8</v>
       </c>
@@ -3884,7 +3928,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
         <v>8</v>
       </c>
@@ -3892,7 +3936,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
         <v>48</v>
       </c>
@@ -4128,7 +4172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C33"/>
   <sheetViews>
@@ -4136,13 +4180,13 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.21875" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>186</v>
       </c>
@@ -4150,7 +4194,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>186</v>
       </c>
@@ -4158,7 +4202,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>186</v>
       </c>
@@ -4166,7 +4210,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>186</v>
       </c>
@@ -4174,7 +4218,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
@@ -4182,7 +4226,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4190,7 +4234,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -4198,7 +4242,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -4206,7 +4250,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>186</v>
       </c>
@@ -4214,7 +4258,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>186</v>
       </c>
@@ -4222,7 +4266,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>186</v>
       </c>
@@ -4230,7 +4274,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>186</v>
       </c>
@@ -4238,7 +4282,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>186</v>
       </c>
@@ -4246,7 +4290,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>186</v>
       </c>
@@ -4254,7 +4298,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>186</v>
       </c>
@@ -4262,7 +4306,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>186</v>
       </c>
@@ -4270,7 +4314,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>186</v>
       </c>
@@ -4278,7 +4322,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>186</v>
       </c>
@@ -4286,7 +4330,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>186</v>
       </c>
@@ -4294,7 +4338,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>186</v>
       </c>
@@ -4302,7 +4346,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>186</v>
       </c>
@@ -4310,7 +4354,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>186</v>
       </c>
@@ -4318,7 +4362,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>186</v>
       </c>
@@ -4326,7 +4370,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>186</v>
       </c>
@@ -4334,7 +4378,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>186</v>
       </c>
@@ -4342,7 +4386,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>186</v>
       </c>
@@ -4350,7 +4394,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>48</v>
       </c>
@@ -4358,7 +4402,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>175</v>
       </c>
@@ -4366,7 +4410,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>186</v>
       </c>
@@ -4374,7 +4418,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>186</v>
       </c>
@@ -4382,7 +4426,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
@@ -4390,7 +4434,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>10</v>
       </c>
@@ -4466,7 +4510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -4474,16 +4518,16 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>305</v>
       </c>
@@ -4497,7 +4541,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>305</v>
       </c>
@@ -4511,7 +4555,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
@@ -4525,7 +4569,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>305</v>
       </c>
@@ -4539,7 +4583,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
@@ -4553,7 +4597,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>311</v>
       </c>
@@ -4570,7 +4614,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>311</v>
       </c>
@@ -4584,7 +4628,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
@@ -4598,7 +4642,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>79</v>
       </c>
@@ -4615,7 +4659,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>79</v>
       </c>
@@ -4632,7 +4676,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
@@ -4646,7 +4690,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>318</v>
       </c>
@@ -4660,7 +4704,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>318</v>
       </c>
@@ -4674,7 +4718,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
@@ -4688,7 +4732,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>24</v>
       </c>
@@ -4702,7 +4746,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
@@ -4719,7 +4763,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>81</v>
       </c>
@@ -4733,7 +4777,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>8</v>
       </c>
@@ -4747,7 +4791,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>8</v>
       </c>
@@ -4761,7 +4805,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>10</v>
       </c>
@@ -4775,7 +4819,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>79</v>
       </c>
@@ -4789,7 +4833,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
         <v>79</v>
       </c>
@@ -4803,7 +4847,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Fix issue with creation of GSettings with unexisting path
</commit_message>
<xml_diff>
--- a/ImplementedFeatures.xlsx
+++ b/ImplementedFeatures.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="364">
   <si>
     <t>GSettings *</t>
   </si>
@@ -1120,6 +1120,9 @@
   </si>
   <si>
     <t>I don't have any sample data in the schema, so can't test</t>
+  </si>
+  <si>
+    <t>Not fully tested</t>
   </si>
 </sst>
 </file>
@@ -1950,7 +1953,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,16 +1992,16 @@
       </c>
       <c r="H2" s="24">
         <f>(I2)/(SUM(I2:I4))</f>
-        <v>0.68518518518518523</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I2" s="21">
         <f>COUNTIF(A:A, 1)</f>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -2009,16 +2012,19 @@
       <c r="D3" s="5" t="s">
         <v>72</v>
       </c>
+      <c r="E3" t="s">
+        <v>363</v>
+      </c>
       <c r="G3" s="28" t="s">
         <v>68</v>
       </c>
       <c r="H3" s="25">
         <f>(I3)/(SUM(I2:I4))</f>
-        <v>7.407407407407407E-2</v>
+        <v>9.2592592592592587E-2</v>
       </c>
       <c r="I3" s="19">
         <f>COUNTIF(A:A, 2)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2096,7 +2102,7 @@
       </c>
       <c r="H7" s="18">
         <f>H2+H3</f>
-        <v>0.7592592592592593</v>
+        <v>0.75925925925925919</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -5236,7 +5242,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5389,9 +5395,6 @@
       </c>
       <c r="E7" t="s">
         <v>327</v>
-      </c>
-      <c r="F7" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>